<commit_message>
updated wish list to add a dummy emial id in sheet myemail
</commit_message>
<xml_diff>
--- a/Package_TataSky_WishList.xlsx
+++ b/Package_TataSky_WishList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MyPack" sheetId="1" r:id="rId1"/>
@@ -1892,7 +1892,7 @@
     <t> insync</t>
   </si>
   <si>
-    <t>venkaeshnarayana15@gmail.com</t>
+    <t>testemail123@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2294,7 +2294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D590"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F181" sqref="F181"/>
     </sheetView>
   </sheetViews>
@@ -11171,7 +11171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>